<commit_message>
Add pivot table to README
</commit_message>
<xml_diff>
--- a/data/Clustering Models/Clustering.xlsx
+++ b/data/Clustering Models/Clustering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wzixu\Desktop\factors-that-affect-median-household-income-in-Baltimore-city\data\Clustering Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44947098-B18F-4B57-8355-BE6B775DB6B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31200EFD-44B4-4977-BAF4-DA1A4EF995D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FEFAC233-E257-47F6-B14B-35AD3F2DEE05}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FEFAC233-E257-47F6-B14B-35AD3F2DEE05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="37">
   <si>
     <t>CT2010</t>
   </si>
@@ -408,16 +408,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>Upper class</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>Upper middle class</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>Middle class</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>Lower class</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -18183,10 +18183,10 @@
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23022,10 +23022,10 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
+        <item n="Upper class" x="0"/>
+        <item n="Upper middle class" x="1"/>
+        <item n="Middle class" x="2"/>
+        <item n="Lower class" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -23378,8 +23378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DFF1D3-80DE-4C81-A22C-67E49A6141CE}">
   <dimension ref="A3:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23400,32 +23400,32 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>1</v>
+      <c r="A4" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B4" s="3">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>2</v>
+      <c r="A5" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B5" s="3">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>3</v>
+      <c r="A6" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B6" s="3">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>4</v>
+      <c r="A7" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B7" s="3">
         <v>64</v>
@@ -23449,7 +23449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7C81F8-91BC-41F4-8391-004E67164647}">
   <dimension ref="A4:AF215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I242" sqref="I242"/>
     </sheetView>
   </sheetViews>

</xml_diff>